<commit_message>
Updating all test cases
</commit_message>
<xml_diff>
--- a/json_to_excel/processing/excel_database.xlsx
+++ b/json_to_excel/processing/excel_database.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Index</t>
   </si>
@@ -82,6 +82,9 @@
     <t>ABC_19</t>
   </si>
   <si>
+    <t>ABC_20</t>
+  </si>
+  <si>
     <t>sample_status_1</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
   </si>
   <si>
     <t>sample_status_19</t>
+  </si>
+  <si>
+    <t>sample_status_20</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -519,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -530,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -541,7 +547,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -552,7 +558,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -563,7 +569,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -574,7 +580,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -585,7 +591,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -596,7 +602,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -607,7 +613,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -618,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -629,7 +635,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -640,7 +646,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -651,7 +657,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -662,7 +668,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -673,7 +679,7 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -684,7 +690,7 @@
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -695,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -706,7 +712,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -717,7 +723,18 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>